<commit_message>
fix gaussian and kmean
</commit_message>
<xml_diff>
--- a/Result/Kmean1.xlsx
+++ b/Result/Kmean1.xlsx
@@ -409,7 +409,7 @@
         <v>0.0006486136563357338</v>
       </c>
       <c r="E2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -428,7 +428,7 @@
         <v>0.0006796754436728395</v>
       </c>
       <c r="E3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -447,7 +447,7 @@
         <v>0.0006503718707133059</v>
       </c>
       <c r="E4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -580,7 +580,7 @@
         <v>0.0004844401752470536</v>
       </c>
       <c r="E11" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12">
@@ -599,7 +599,7 @@
         <v>0.0005060923546373283</v>
       </c>
       <c r="E12" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13">
@@ -618,7 +618,7 @@
         <v>0.0005217300397525267</v>
       </c>
       <c r="E13" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14">
@@ -713,7 +713,7 @@
         <v>0.001011445473251029</v>
       </c>
       <c r="E18" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19">
@@ -732,7 +732,7 @@
         <v>0.0005088305898491084</v>
       </c>
       <c r="E19" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20">
@@ -751,7 +751,7 @@
         <v>0.0001133830589849108</v>
       </c>
       <c r="E20" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21">
@@ -770,7 +770,7 @@
         <v>9.409293552812072e-05</v>
       </c>
       <c r="E21" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22">
@@ -789,7 +789,7 @@
         <v>9.194958847736624e-05</v>
       </c>
       <c r="E22" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23">
@@ -960,7 +960,7 @@
         <v>0.0004969999999999999</v>
       </c>
       <c r="E31" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32">
@@ -1036,7 +1036,7 @@
         <v>0.0005789180384087793</v>
       </c>
       <c r="E35" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="36">
@@ -1055,7 +1055,7 @@
         <v>0.0004942558299039781</v>
       </c>
       <c r="E36" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="37">
@@ -1074,7 +1074,7 @@
         <v>0.0005949931412894375</v>
       </c>
       <c r="E37" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="38">
@@ -1093,7 +1093,7 @@
         <v>0.0007145919067215363</v>
       </c>
       <c r="E38" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="39">
@@ -1112,7 +1112,7 @@
         <v>0.0007302383401920438</v>
       </c>
       <c r="E39" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="40">
@@ -1131,7 +1131,7 @@
         <v>0.0007210219478737997</v>
       </c>
       <c r="E40" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="41">
@@ -1150,7 +1150,7 @@
         <v>0.0005561985596707819</v>
       </c>
       <c r="E41" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="42">
@@ -1169,7 +1169,7 @@
         <v>0.00064900548696845</v>
       </c>
       <c r="E42" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="43">
@@ -1188,7 +1188,7 @@
         <v>0.0006024948559670782</v>
       </c>
       <c r="E43" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="44">
@@ -1207,7 +1207,7 @@
         <v>0.000482681755829904</v>
       </c>
       <c r="E44" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45">
@@ -1226,7 +1226,7 @@
         <v>0.0005199759945130316</v>
       </c>
       <c r="E45" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46">
@@ -1245,7 +1245,7 @@
         <v>0.0004355281207133059</v>
       </c>
       <c r="E46" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47">
@@ -1283,7 +1283,7 @@
         <v>0.0001736111111111111</v>
       </c>
       <c r="E48" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="49">
@@ -1302,7 +1302,7 @@
         <v>0.0001718964334705076</v>
       </c>
       <c r="E49" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="50">
@@ -1321,7 +1321,7 @@
         <v>0.000128</v>
       </c>
       <c r="E50" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="51">
@@ -1340,7 +1340,7 @@
         <v>0.000229</v>
       </c>
       <c r="E51" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="52">
@@ -1359,7 +1359,7 @@
         <v>0.000136</v>
       </c>
       <c r="E52" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="53">
@@ -1378,7 +1378,7 @@
         <v>0.0004944701646090535</v>
       </c>
       <c r="E53" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="54">
@@ -1397,7 +1397,7 @@
         <v>0.0005268347050754458</v>
       </c>
       <c r="E54" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="55">
@@ -1416,7 +1416,7 @@
         <v>0.0006187842935528121</v>
       </c>
       <c r="E55" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="56">
@@ -1435,7 +1435,7 @@
         <v>0.0002580589849108368</v>
       </c>
       <c r="E56" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57">
@@ -1454,7 +1454,7 @@
         <v>0.0002593449931412894</v>
       </c>
       <c r="E57" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58">
@@ -1473,7 +1473,7 @@
         <v>0.0004001628943758574</v>
       </c>
       <c r="E58" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59">
@@ -1492,7 +1492,7 @@
         <v>0.0004565329218106996</v>
       </c>
       <c r="E59" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60">
@@ -1511,7 +1511,7 @@
         <v>0.000524048353909465</v>
       </c>
       <c r="E60" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61">
@@ -1530,7 +1530,7 @@
         <v>0.0005225480109739369</v>
       </c>
       <c r="E61" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62">
@@ -1549,7 +1549,7 @@
         <v>6.515775034293553e-05</v>
       </c>
       <c r="E62" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="63">
@@ -1568,7 +1568,7 @@
         <v>7.051611796982167e-05</v>
       </c>
       <c r="E63" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="64">
@@ -1587,7 +1587,7 @@
         <v>2.593449931412895e-05</v>
       </c>
       <c r="E64" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="65">
@@ -1606,7 +1606,7 @@
         <v>0.0003099279835390947</v>
       </c>
       <c r="E65" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66">
@@ -1625,7 +1625,7 @@
         <v>0.0004301697530864198</v>
       </c>
       <c r="E66" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67">
@@ -1644,7 +1644,7 @@
         <v>0.000391803840877915</v>
       </c>
       <c r="E67" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68">
@@ -1663,7 +1663,7 @@
         <v>0.0001033093278463649</v>
       </c>
       <c r="E68" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="69">
@@ -1682,7 +1682,7 @@
         <v>0.0001371742112482853</v>
       </c>
       <c r="E69" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="70">
@@ -1701,7 +1701,7 @@
         <v>0.0001043810013717421</v>
       </c>
       <c r="E70" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="71">
@@ -1777,7 +1777,7 @@
         <v>0</v>
       </c>
       <c r="E74" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="75">
@@ -1796,7 +1796,7 @@
         <v>0</v>
       </c>
       <c r="E75" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="76">
@@ -1815,7 +1815,7 @@
         <v>0</v>
       </c>
       <c r="E76" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="77">
@@ -1834,7 +1834,7 @@
         <v>0.0005977794924554182</v>
       </c>
       <c r="E77" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="78">
@@ -1853,7 +1853,7 @@
         <v>0.0007600308641975309</v>
       </c>
       <c r="E78" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="79">
@@ -1872,7 +1872,7 @@
         <v>0.0007188786008230452</v>
       </c>
       <c r="E79" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="80">
@@ -1891,7 +1891,7 @@
         <v>0.0008547668038408777</v>
       </c>
       <c r="E80" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="81">
@@ -1910,7 +1910,7 @@
         <v>0.0008667695473251028</v>
       </c>
       <c r="E81" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="82">
@@ -1929,7 +1929,7 @@
         <v>0.001069101508916324</v>
       </c>
       <c r="E82" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="83">

</xml_diff>